<commit_message>
add Greener scenario's land use table and emission for comparison
</commit_message>
<xml_diff>
--- a/data_dir/provinces/Jambi/compile_lcArea.xlsx
+++ b/data_dir/provinces/Jambi/compile_lcArea.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PPRK\process\projects\2019_07\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PPRK\process\PPRK_git\pprk_apps\data_dir\provinces\Jambi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA2A9B5F-59F1-4226-846D-9CEA504EFD2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82507C24-EE9A-48BC-9656-3EB4CFD30910}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="compile_lcArea" sheetId="1" r:id="rId1"/>
+    <sheet name="compile_lcArea_Green" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
   <si>
     <t>value</t>
   </si>
@@ -155,12 +163,18 @@
   </si>
   <si>
     <t>Awan</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Land_use_type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -994,10 +1008,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2636,4 +2650,1174 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1B1665-B2FF-403E-B089-521CCF50197D}">
+  <dimension ref="A1:P23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:P24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>580931</v>
+      </c>
+      <c r="D2">
+        <v>580932</v>
+      </c>
+      <c r="E2">
+        <v>580948</v>
+      </c>
+      <c r="F2">
+        <v>580954</v>
+      </c>
+      <c r="G2">
+        <v>580961</v>
+      </c>
+      <c r="H2">
+        <v>580971</v>
+      </c>
+      <c r="I2">
+        <v>580981</v>
+      </c>
+      <c r="J2">
+        <v>580993</v>
+      </c>
+      <c r="K2">
+        <v>581000</v>
+      </c>
+      <c r="L2">
+        <v>581007</v>
+      </c>
+      <c r="M2">
+        <v>581008</v>
+      </c>
+      <c r="N2">
+        <v>581009</v>
+      </c>
+      <c r="O2">
+        <v>581008</v>
+      </c>
+      <c r="P2">
+        <v>581011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>289816</v>
+      </c>
+      <c r="D3">
+        <v>291556</v>
+      </c>
+      <c r="E3">
+        <v>293204</v>
+      </c>
+      <c r="F3">
+        <v>294841</v>
+      </c>
+      <c r="G3">
+        <v>296452</v>
+      </c>
+      <c r="H3">
+        <v>297813</v>
+      </c>
+      <c r="I3">
+        <v>299130</v>
+      </c>
+      <c r="J3">
+        <v>300349</v>
+      </c>
+      <c r="K3">
+        <v>301415</v>
+      </c>
+      <c r="L3">
+        <v>302366</v>
+      </c>
+      <c r="M3">
+        <v>303277</v>
+      </c>
+      <c r="N3">
+        <v>304112</v>
+      </c>
+      <c r="O3">
+        <v>304909</v>
+      </c>
+      <c r="P3">
+        <v>305577</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>132451</v>
+      </c>
+      <c r="D4">
+        <v>132519</v>
+      </c>
+      <c r="E4">
+        <v>132578</v>
+      </c>
+      <c r="F4">
+        <v>132633</v>
+      </c>
+      <c r="G4">
+        <v>132683</v>
+      </c>
+      <c r="H4">
+        <v>132732</v>
+      </c>
+      <c r="I4">
+        <v>132773</v>
+      </c>
+      <c r="J4">
+        <v>132819</v>
+      </c>
+      <c r="K4">
+        <v>132865</v>
+      </c>
+      <c r="L4">
+        <v>132913</v>
+      </c>
+      <c r="M4">
+        <v>132952</v>
+      </c>
+      <c r="N4">
+        <v>132989</v>
+      </c>
+      <c r="O4">
+        <v>133031</v>
+      </c>
+      <c r="P4">
+        <v>133066</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>46117</v>
+      </c>
+      <c r="D5">
+        <v>47799</v>
+      </c>
+      <c r="E5">
+        <v>48935</v>
+      </c>
+      <c r="F5">
+        <v>49821</v>
+      </c>
+      <c r="G5">
+        <v>50483</v>
+      </c>
+      <c r="H5">
+        <v>51147</v>
+      </c>
+      <c r="I5">
+        <v>51592</v>
+      </c>
+      <c r="J5">
+        <v>52082</v>
+      </c>
+      <c r="K5">
+        <v>52397</v>
+      </c>
+      <c r="L5">
+        <v>52638</v>
+      </c>
+      <c r="M5">
+        <v>52909</v>
+      </c>
+      <c r="N5">
+        <v>53177</v>
+      </c>
+      <c r="O5">
+        <v>53405</v>
+      </c>
+      <c r="P5">
+        <v>53589</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>805</v>
+      </c>
+      <c r="D6">
+        <v>805</v>
+      </c>
+      <c r="E6">
+        <v>805</v>
+      </c>
+      <c r="F6">
+        <v>805</v>
+      </c>
+      <c r="G6">
+        <v>805</v>
+      </c>
+      <c r="H6">
+        <v>805</v>
+      </c>
+      <c r="I6">
+        <v>805</v>
+      </c>
+      <c r="J6">
+        <v>805</v>
+      </c>
+      <c r="K6">
+        <v>805</v>
+      </c>
+      <c r="L6">
+        <v>805</v>
+      </c>
+      <c r="M6">
+        <v>805</v>
+      </c>
+      <c r="N6">
+        <v>805</v>
+      </c>
+      <c r="O6">
+        <v>805</v>
+      </c>
+      <c r="P6">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>4095</v>
+      </c>
+      <c r="D7">
+        <v>4131</v>
+      </c>
+      <c r="E7">
+        <v>4158</v>
+      </c>
+      <c r="F7">
+        <v>4183</v>
+      </c>
+      <c r="G7">
+        <v>4210</v>
+      </c>
+      <c r="H7">
+        <v>4240</v>
+      </c>
+      <c r="I7">
+        <v>4272</v>
+      </c>
+      <c r="J7">
+        <v>4301</v>
+      </c>
+      <c r="K7">
+        <v>4331</v>
+      </c>
+      <c r="L7">
+        <v>4352</v>
+      </c>
+      <c r="M7">
+        <v>4369</v>
+      </c>
+      <c r="N7">
+        <v>4390</v>
+      </c>
+      <c r="O7">
+        <v>4409</v>
+      </c>
+      <c r="P7">
+        <v>4424</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>240037</v>
+      </c>
+      <c r="D8">
+        <v>227663</v>
+      </c>
+      <c r="E8">
+        <v>220199</v>
+      </c>
+      <c r="F8">
+        <v>215492</v>
+      </c>
+      <c r="G8">
+        <v>212109</v>
+      </c>
+      <c r="H8">
+        <v>208711</v>
+      </c>
+      <c r="I8">
+        <v>205998</v>
+      </c>
+      <c r="J8">
+        <v>203884</v>
+      </c>
+      <c r="K8">
+        <v>202420</v>
+      </c>
+      <c r="L8">
+        <v>201073</v>
+      </c>
+      <c r="M8">
+        <v>199989</v>
+      </c>
+      <c r="N8">
+        <v>198965</v>
+      </c>
+      <c r="O8">
+        <v>198134</v>
+      </c>
+      <c r="P8">
+        <v>197282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9">
+        <v>445750</v>
+      </c>
+      <c r="D9">
+        <v>525344</v>
+      </c>
+      <c r="E9">
+        <v>595960</v>
+      </c>
+      <c r="F9">
+        <v>652318</v>
+      </c>
+      <c r="G9">
+        <v>697784</v>
+      </c>
+      <c r="H9">
+        <v>734554</v>
+      </c>
+      <c r="I9">
+        <v>758878</v>
+      </c>
+      <c r="J9">
+        <v>761648</v>
+      </c>
+      <c r="K9">
+        <v>760831</v>
+      </c>
+      <c r="L9">
+        <v>755408</v>
+      </c>
+      <c r="M9">
+        <v>755820</v>
+      </c>
+      <c r="N9">
+        <v>754589</v>
+      </c>
+      <c r="O9">
+        <v>754729</v>
+      </c>
+      <c r="P9">
+        <v>753455</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>208972</v>
+      </c>
+      <c r="D10">
+        <v>201669</v>
+      </c>
+      <c r="E10">
+        <v>195233</v>
+      </c>
+      <c r="F10">
+        <v>190723</v>
+      </c>
+      <c r="G10">
+        <v>187554</v>
+      </c>
+      <c r="H10">
+        <v>185074</v>
+      </c>
+      <c r="I10">
+        <v>183548</v>
+      </c>
+      <c r="J10">
+        <v>182129</v>
+      </c>
+      <c r="K10">
+        <v>181197</v>
+      </c>
+      <c r="L10">
+        <v>180317</v>
+      </c>
+      <c r="M10">
+        <v>179820</v>
+      </c>
+      <c r="N10">
+        <v>179095</v>
+      </c>
+      <c r="O10">
+        <v>178850</v>
+      </c>
+      <c r="P10">
+        <v>178001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11">
+        <v>92</v>
+      </c>
+      <c r="D11">
+        <v>92</v>
+      </c>
+      <c r="E11">
+        <v>92</v>
+      </c>
+      <c r="F11">
+        <v>92</v>
+      </c>
+      <c r="G11">
+        <v>92</v>
+      </c>
+      <c r="H11">
+        <v>92</v>
+      </c>
+      <c r="I11">
+        <v>92</v>
+      </c>
+      <c r="J11">
+        <v>92</v>
+      </c>
+      <c r="K11">
+        <v>92</v>
+      </c>
+      <c r="L11">
+        <v>92</v>
+      </c>
+      <c r="M11">
+        <v>92</v>
+      </c>
+      <c r="N11">
+        <v>92</v>
+      </c>
+      <c r="O11">
+        <v>92</v>
+      </c>
+      <c r="P11">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>971225</v>
+      </c>
+      <c r="D12">
+        <v>1005990</v>
+      </c>
+      <c r="E12">
+        <v>1037350</v>
+      </c>
+      <c r="F12">
+        <v>1065482</v>
+      </c>
+      <c r="G12">
+        <v>1090864</v>
+      </c>
+      <c r="H12">
+        <v>1113844</v>
+      </c>
+      <c r="I12">
+        <v>1134115</v>
+      </c>
+      <c r="J12">
+        <v>1152914</v>
+      </c>
+      <c r="K12">
+        <v>1169050</v>
+      </c>
+      <c r="L12">
+        <v>1177086</v>
+      </c>
+      <c r="M12">
+        <v>1180765</v>
+      </c>
+      <c r="N12">
+        <v>1183927</v>
+      </c>
+      <c r="O12">
+        <v>1185524</v>
+      </c>
+      <c r="P12">
+        <v>1184392</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>98692</v>
+      </c>
+      <c r="D13">
+        <v>94558</v>
+      </c>
+      <c r="E13">
+        <v>92074</v>
+      </c>
+      <c r="F13">
+        <v>90592</v>
+      </c>
+      <c r="G13">
+        <v>89668</v>
+      </c>
+      <c r="H13">
+        <v>89235</v>
+      </c>
+      <c r="I13">
+        <v>89828</v>
+      </c>
+      <c r="J13">
+        <v>90489</v>
+      </c>
+      <c r="K13">
+        <v>90784</v>
+      </c>
+      <c r="L13">
+        <v>90948</v>
+      </c>
+      <c r="M13">
+        <v>91174</v>
+      </c>
+      <c r="N13">
+        <v>91453</v>
+      </c>
+      <c r="O13">
+        <v>91734</v>
+      </c>
+      <c r="P13">
+        <v>92030</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>1433560</v>
+      </c>
+      <c r="D14">
+        <v>1330873</v>
+      </c>
+      <c r="E14">
+        <v>1236890</v>
+      </c>
+      <c r="F14">
+        <v>1156903</v>
+      </c>
+      <c r="G14">
+        <v>1089073</v>
+      </c>
+      <c r="H14">
+        <v>1029728</v>
+      </c>
+      <c r="I14">
+        <v>983410</v>
+      </c>
+      <c r="J14">
+        <v>959276</v>
+      </c>
+      <c r="K14">
+        <v>941246</v>
+      </c>
+      <c r="L14">
+        <v>935378</v>
+      </c>
+      <c r="M14">
+        <v>927912</v>
+      </c>
+      <c r="N14">
+        <v>922205</v>
+      </c>
+      <c r="O14">
+        <v>916606</v>
+      </c>
+      <c r="P14">
+        <v>915315</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15">
+        <v>21839</v>
+      </c>
+      <c r="D15">
+        <v>21841</v>
+      </c>
+      <c r="E15">
+        <v>21844</v>
+      </c>
+      <c r="F15">
+        <v>21848</v>
+      </c>
+      <c r="G15">
+        <v>21852</v>
+      </c>
+      <c r="H15">
+        <v>21857</v>
+      </c>
+      <c r="I15">
+        <v>21863</v>
+      </c>
+      <c r="J15">
+        <v>21869</v>
+      </c>
+      <c r="K15">
+        <v>21875</v>
+      </c>
+      <c r="L15">
+        <v>21881</v>
+      </c>
+      <c r="M15">
+        <v>21886</v>
+      </c>
+      <c r="N15">
+        <v>21892</v>
+      </c>
+      <c r="O15">
+        <v>21898</v>
+      </c>
+      <c r="P15">
+        <v>21904</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>16925</v>
+      </c>
+      <c r="D16">
+        <v>16980</v>
+      </c>
+      <c r="E16">
+        <v>17132</v>
+      </c>
+      <c r="F16">
+        <v>17319</v>
+      </c>
+      <c r="G16">
+        <v>17517</v>
+      </c>
+      <c r="H16">
+        <v>17712</v>
+      </c>
+      <c r="I16">
+        <v>17876</v>
+      </c>
+      <c r="J16">
+        <v>18022</v>
+      </c>
+      <c r="K16">
+        <v>18173</v>
+      </c>
+      <c r="L16">
+        <v>18336</v>
+      </c>
+      <c r="M16">
+        <v>18504</v>
+      </c>
+      <c r="N16">
+        <v>18664</v>
+      </c>
+      <c r="O16">
+        <v>18825</v>
+      </c>
+      <c r="P16">
+        <v>18998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <v>200</v>
+      </c>
+      <c r="D17">
+        <v>197</v>
+      </c>
+      <c r="E17">
+        <v>197</v>
+      </c>
+      <c r="F17">
+        <v>197</v>
+      </c>
+      <c r="G17">
+        <v>197</v>
+      </c>
+      <c r="H17">
+        <v>197</v>
+      </c>
+      <c r="I17">
+        <v>197</v>
+      </c>
+      <c r="J17">
+        <v>197</v>
+      </c>
+      <c r="K17">
+        <v>197</v>
+      </c>
+      <c r="L17">
+        <v>197</v>
+      </c>
+      <c r="M17">
+        <v>197</v>
+      </c>
+      <c r="N17">
+        <v>197</v>
+      </c>
+      <c r="O17">
+        <v>197</v>
+      </c>
+      <c r="P17">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18">
+        <v>233977</v>
+      </c>
+      <c r="D18">
+        <v>237058</v>
+      </c>
+      <c r="E18">
+        <v>237216</v>
+      </c>
+      <c r="F18">
+        <v>235812</v>
+      </c>
+      <c r="G18">
+        <v>233219</v>
+      </c>
+      <c r="H18">
+        <v>232585</v>
+      </c>
+      <c r="I18">
+        <v>231818</v>
+      </c>
+      <c r="J18">
+        <v>230980</v>
+      </c>
+      <c r="K18">
+        <v>229466</v>
+      </c>
+      <c r="L18">
+        <v>228441</v>
+      </c>
+      <c r="M18">
+        <v>226972</v>
+      </c>
+      <c r="N18">
+        <v>226220</v>
+      </c>
+      <c r="O18">
+        <v>225047</v>
+      </c>
+      <c r="P18">
+        <v>224628</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19">
+        <v>14568</v>
+      </c>
+      <c r="D19">
+        <v>15569</v>
+      </c>
+      <c r="E19">
+        <v>16482</v>
+      </c>
+      <c r="F19">
+        <v>17363</v>
+      </c>
+      <c r="G19">
+        <v>18234</v>
+      </c>
+      <c r="H19">
+        <v>19045</v>
+      </c>
+      <c r="I19">
+        <v>19820</v>
+      </c>
+      <c r="J19">
+        <v>20560</v>
+      </c>
+      <c r="K19">
+        <v>21275</v>
+      </c>
+      <c r="L19">
+        <v>21977</v>
+      </c>
+      <c r="M19">
+        <v>22666</v>
+      </c>
+      <c r="N19">
+        <v>23348</v>
+      </c>
+      <c r="O19">
+        <v>24015</v>
+      </c>
+      <c r="P19">
+        <v>24664</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>91209</v>
+      </c>
+      <c r="D20">
+        <v>95745</v>
+      </c>
+      <c r="E20">
+        <v>100082</v>
+      </c>
+      <c r="F20">
+        <v>104058</v>
+      </c>
+      <c r="G20">
+        <v>107735</v>
+      </c>
+      <c r="H20">
+        <v>111205</v>
+      </c>
+      <c r="I20">
+        <v>114605</v>
+      </c>
+      <c r="J20">
+        <v>118245</v>
+      </c>
+      <c r="K20">
+        <v>122287</v>
+      </c>
+      <c r="L20">
+        <v>126542</v>
+      </c>
+      <c r="M20">
+        <v>130690</v>
+      </c>
+      <c r="N20">
+        <v>134728</v>
+      </c>
+      <c r="O20">
+        <v>138686</v>
+      </c>
+      <c r="P20">
+        <v>142520</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21">
+        <v>43564</v>
+      </c>
+      <c r="D21">
+        <v>43564</v>
+      </c>
+      <c r="E21">
+        <v>43564</v>
+      </c>
+      <c r="F21">
+        <v>43564</v>
+      </c>
+      <c r="G21">
+        <v>43564</v>
+      </c>
+      <c r="H21">
+        <v>43564</v>
+      </c>
+      <c r="I21">
+        <v>43564</v>
+      </c>
+      <c r="J21">
+        <v>43564</v>
+      </c>
+      <c r="K21">
+        <v>43564</v>
+      </c>
+      <c r="L21">
+        <v>43564</v>
+      </c>
+      <c r="M21">
+        <v>43564</v>
+      </c>
+      <c r="N21">
+        <v>43564</v>
+      </c>
+      <c r="O21">
+        <v>43564</v>
+      </c>
+      <c r="P21">
+        <v>43564</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22">
+        <v>15141</v>
+      </c>
+      <c r="D22">
+        <v>15081</v>
+      </c>
+      <c r="E22">
+        <v>15023</v>
+      </c>
+      <c r="F22">
+        <v>14966</v>
+      </c>
+      <c r="G22">
+        <v>14910</v>
+      </c>
+      <c r="H22">
+        <v>14855</v>
+      </c>
+      <c r="I22">
+        <v>14801</v>
+      </c>
+      <c r="J22">
+        <v>14748</v>
+      </c>
+      <c r="K22">
+        <v>14696</v>
+      </c>
+      <c r="L22">
+        <v>14645</v>
+      </c>
+      <c r="M22">
+        <v>14595</v>
+      </c>
+      <c r="N22">
+        <v>14545</v>
+      </c>
+      <c r="O22">
+        <v>14498</v>
+      </c>
+      <c r="P22">
+        <v>14452</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23">
+        <v>81</v>
+      </c>
+      <c r="D23">
+        <v>81</v>
+      </c>
+      <c r="E23">
+        <v>81</v>
+      </c>
+      <c r="F23">
+        <v>81</v>
+      </c>
+      <c r="G23">
+        <v>81</v>
+      </c>
+      <c r="H23">
+        <v>81</v>
+      </c>
+      <c r="I23">
+        <v>81</v>
+      </c>
+      <c r="J23">
+        <v>81</v>
+      </c>
+      <c r="K23">
+        <v>81</v>
+      </c>
+      <c r="L23">
+        <v>81</v>
+      </c>
+      <c r="M23">
+        <v>81</v>
+      </c>
+      <c r="N23">
+        <v>81</v>
+      </c>
+      <c r="O23">
+        <v>81</v>
+      </c>
+      <c r="P23">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>